<commit_message>
3.4.2 --> 3.4.3 updating io-model/FtPICM (splits natural gas revenue between production & distribution, using U.S. data for lack of granularity in EU use tables)
</commit_message>
<xml_diff>
--- a/InputData/io-model/FtPICM/Fuel to Producing ISIC Code Map.xlsx
+++ b/InputData/io-model/FtPICM/Fuel to Producing ISIC Code Map.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\eps-eu\InputData\io-model\FtPICM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\E.U. Models\eps-eu\InputData\io-model\FtPICM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6716CA9E-8FB3-4F7C-8A84-AA79007037A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E46D97-79AE-4627-8318-CA536CA75873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27600" yWindow="1455" windowWidth="25995" windowHeight="13605" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="59115" yWindow="1245" windowWidth="24240" windowHeight="13590" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="Pre ISIC Consolidation" sheetId="3" r:id="rId2"/>
-    <sheet name="FtPICM" sheetId="2" r:id="rId3"/>
+    <sheet name="Fuel Transport Calcs" sheetId="5" r:id="rId2"/>
+    <sheet name="Pre ISIC Consolidation" sheetId="3" r:id="rId3"/>
+    <sheet name="FtPICM" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,14 +39,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="102">
   <si>
     <t>Source:</t>
   </si>
   <si>
-    <t>none needed</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -266,13 +264,94 @@
   </si>
   <si>
     <t>EU ISIC Groupings</t>
+  </si>
+  <si>
+    <t>We need to divide up revenue from selling "natural gas" between the</t>
+  </si>
+  <si>
+    <t>oil and gas extraction ISIC code and the "energy pipelines and gas processing"</t>
+  </si>
+  <si>
+    <t>ISIC code.</t>
+  </si>
+  <si>
+    <t>Oil and Gas Extraction Revenue</t>
+  </si>
+  <si>
+    <t>million $</t>
+  </si>
+  <si>
+    <t>Share of oil and gas revenue from natural gas</t>
+  </si>
+  <si>
+    <t>https://www.eia.gov/todayinenergy/detail.php?id=49776</t>
+  </si>
+  <si>
+    <t>Gas Revenue</t>
+  </si>
+  <si>
+    <t>Revenue received from NG distribution companies</t>
+  </si>
+  <si>
+    <t>Revenue received from pipeline transportation companies</t>
+  </si>
+  <si>
+    <t>Share of pipeline transportation revenue attributable to transport of natural gas</t>
+  </si>
+  <si>
+    <t>Total revenue for NG transport and distribution</t>
+  </si>
+  <si>
+    <t>Share of NG revenue for transport and distribution</t>
+  </si>
+  <si>
+    <t>According to the BEA "Use Table" data, no appreciable share of oil revenue goes to transport.</t>
+  </si>
+  <si>
+    <t>Therefore, we only need to split up revenue for natural gas, not for crude oil or secondary petroleum products.</t>
+  </si>
+  <si>
+    <t>Splitting natural gas revenue between production and transmission/distribution</t>
+  </si>
+  <si>
+    <t>U.S. Bureau of Economic Analysis</t>
+  </si>
+  <si>
+    <t>Input-Output Accounts Data</t>
+  </si>
+  <si>
+    <t>https://www.bea.gov/industry/input-output-accounts-data</t>
+  </si>
+  <si>
+    <t>"Use of Commodities by Industry" table, 405-industry breakdown</t>
+  </si>
+  <si>
+    <t>"energy pipelines and gas processing" ISIC code.  (We don't need to do anything similar for oil</t>
+  </si>
+  <si>
+    <t>in this variable because no appreciable portion of the revenue goes to transport, and we already assign</t>
+  </si>
+  <si>
+    <t>crude oil to extraction and secondary petroleum products to refineries, so it's already handled by</t>
+  </si>
+  <si>
+    <t>the use of different fuel types.)</t>
+  </si>
+  <si>
+    <t>We use U.S. BEA data to divide up natural gas revenue between the "oil and gas extraction" ISIC code and the</t>
+  </si>
+  <si>
+    <t>EU use table data is broken into different product &amp; industry groupings, not allowing the same level of</t>
+  </si>
+  <si>
+    <t xml:space="preserve">commodity breakdown as the U.S. file allows. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -296,8 +375,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -316,6 +407,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -326,10 +429,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -340,10 +445,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{8DFCED53-43D2-45FB-884A-785D98AFB383}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -647,7 +763,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -655,205 +771,420 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="70.6328125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B5" s="12">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B7" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{7057CE15-EA2E-42A5-913B-C44144EF70CB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE09666E-1109-4373-939A-48507479F2F3}">
+  <dimension ref="A1:C32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="6">
+        <v>683995</v>
+      </c>
+      <c r="B7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="7">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="9">
+        <v>95759.3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="6">
+        <v>18217</v>
+      </c>
+      <c r="B16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="6">
+        <v>61</v>
+      </c>
+      <c r="B19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>8.5400000000000009</v>
+      </c>
+      <c r="B21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="6">
+        <v>18225.54</v>
+      </c>
+      <c r="B24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="10">
+        <v>0.19032657924608889</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C10" r:id="rId1" xr:uid="{A5277234-F72C-43C8-B1B2-415E053D3207}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AQ26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V12" sqref="A6:V12"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:43" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AN1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AO1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AP1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="AQ1" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -984,7 +1315,7 @@
     </row>
     <row r="3" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1115,7 +1446,7 @@
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1123,8 +1454,9 @@
       <c r="C4">
         <v>0</v>
       </c>
-      <c r="D4">
-        <v>0</v>
+      <c r="D4" s="13">
+        <f>1-AA4</f>
+        <v>0.80967342075391113</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -1192,8 +1524,9 @@
       <c r="Z4">
         <v>0</v>
       </c>
-      <c r="AA4" s="4">
-        <v>1</v>
+      <c r="AA4" s="13">
+        <f>'Fuel Transport Calcs'!A27</f>
+        <v>0.19032657924608889</v>
       </c>
       <c r="AB4">
         <v>0</v>
@@ -1246,7 +1579,7 @@
     </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1377,7 +1710,7 @@
     </row>
     <row r="6" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1508,7 +1841,7 @@
     </row>
     <row r="7" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1639,7 +1972,7 @@
     </row>
     <row r="8" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -1770,7 +2103,7 @@
     </row>
     <row r="9" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9" s="4">
         <v>1</v>
@@ -1901,7 +2234,7 @@
     </row>
     <row r="10" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -2032,7 +2365,7 @@
     </row>
     <row r="11" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -2163,7 +2496,7 @@
     </row>
     <row r="12" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -2294,7 +2627,7 @@
     </row>
     <row r="13" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -2425,7 +2758,7 @@
     </row>
     <row r="14" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -2556,7 +2889,7 @@
     </row>
     <row r="15" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -2687,7 +3020,7 @@
     </row>
     <row r="16" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -2818,7 +3151,7 @@
     </row>
     <row r="17" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -2949,7 +3282,7 @@
     </row>
     <row r="18" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -3080,7 +3413,7 @@
     </row>
     <row r="19" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -3211,7 +3544,7 @@
     </row>
     <row r="20" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -3342,7 +3675,7 @@
     </row>
     <row r="21" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -3473,7 +3806,7 @@
     </row>
     <row r="22" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -3604,7 +3937,7 @@
     </row>
     <row r="24" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -3651,264 +3984,264 @@
     </row>
     <row r="25" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B25" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="D25" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="E25" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="F25" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="G25" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="H25" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="I25" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I25" s="3" t="s">
+      <c r="J25" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J25" s="3" t="s">
+      <c r="K25" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K25" s="3" t="s">
+      <c r="L25" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L25" s="3" t="s">
+      <c r="M25" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="M25" s="3" t="s">
+      <c r="N25" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="N25" s="3" t="s">
+      <c r="O25" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="O25" s="3" t="s">
+      <c r="P25" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="P25" s="3" t="s">
+      <c r="Q25" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="Q25" s="3" t="s">
+      <c r="R25" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="R25" s="3" t="s">
+      <c r="S25" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="S25" s="3" t="s">
+      <c r="T25" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="T25" s="3" t="s">
+      <c r="U25" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="U25" s="3" t="s">
+      <c r="V25" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="V25" s="3" t="s">
+      <c r="W25" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="W25" s="3" t="s">
+      <c r="X25" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="X25" s="3" t="s">
+      <c r="Y25" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="Y25" s="3" t="s">
+      <c r="Z25" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="Z25" s="3" t="s">
+      <c r="AA25" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AA25" s="3" t="s">
+      <c r="AB25" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AB25" s="3" t="s">
+      <c r="AC25" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AC25" s="3" t="s">
+      <c r="AD25" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AD25" s="3" t="s">
+      <c r="AE25" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AE25" s="3" t="s">
+      <c r="AF25" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AF25" s="3" t="s">
+      <c r="AG25" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AG25" s="3" t="s">
+      <c r="AH25" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AH25" s="3" t="s">
+      <c r="AI25" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AI25" s="3" t="s">
+      <c r="AJ25" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AJ25" s="3" t="s">
+      <c r="AK25" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AK25" s="3" t="s">
+      <c r="AL25" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AL25" s="3" t="s">
+      <c r="AM25" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AM25" s="3" t="s">
+      <c r="AN25" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AN25" s="3" t="s">
+      <c r="AO25" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AO25" s="3" t="s">
+      <c r="AP25" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="AP25" s="3" t="s">
+      <c r="AQ25" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="AQ25" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="F26" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="G26" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="H26" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H26" s="3" t="s">
+      <c r="I26" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I26" s="3" t="s">
+      <c r="J26" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J26" s="3" t="s">
+      <c r="K26" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K26" s="3" t="s">
+      <c r="L26" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L26" s="3" t="s">
+      <c r="M26" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="M26" s="3" t="s">
+      <c r="N26" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="N26" s="3" t="s">
+      <c r="O26" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="O26" s="3" t="s">
+      <c r="P26" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="P26" s="3" t="s">
+      <c r="Q26" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="Q26" s="3" t="s">
+      <c r="R26" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="R26" s="3" t="s">
+      <c r="S26" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="S26" s="3" t="s">
+      <c r="T26" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="T26" s="3" t="s">
+      <c r="U26" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="U26" s="3" t="s">
+      <c r="V26" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="V26" s="3" t="s">
+      <c r="W26" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="W26" s="3" t="s">
+      <c r="X26" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="X26" s="3" t="s">
+      <c r="Y26" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="Y26" s="3" t="s">
+      <c r="Z26" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="Z26" s="3" t="s">
+      <c r="AA26" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AA26" s="3" t="s">
+      <c r="AB26" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AB26" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="AC26" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AD26" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE26" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AE26" s="3" t="s">
+      <c r="AF26" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AF26" s="3" t="s">
+      <c r="AG26" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AG26" s="3" t="s">
+      <c r="AH26" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AH26" s="3" t="s">
+      <c r="AI26" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AI26" s="3" t="s">
+      <c r="AJ26" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AJ26" s="3" t="s">
+      <c r="AK26" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AK26" s="3" t="s">
+      <c r="AL26" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AL26" s="3" t="s">
+      <c r="AM26" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AM26" s="3" t="s">
+      <c r="AN26" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AN26" s="3" t="s">
+      <c r="AO26" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AO26" s="3" t="s">
+      <c r="AP26" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="AP26" s="3" t="s">
+      <c r="AQ26" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="AQ26" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -3916,7 +4249,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
@@ -3924,10 +4257,10 @@
   <dimension ref="A1:AQ22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y5" sqref="Y5"/>
+      <selection pane="bottomRight" activeCell="AA4" sqref="AA4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3938,138 +4271,138 @@
   <sheetData>
     <row r="1" spans="1:43" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AN1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AO1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AP1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="AQ1" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2">
         <f>SUMIFS('Pre ISIC Consolidation'!$B2:$AQ2,'Pre ISIC Consolidation'!$B$26:$AQ$26,FtPICM!B$1)</f>
@@ -4242,7 +4575,7 @@
     </row>
     <row r="3" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3">
         <f>SUMIFS('Pre ISIC Consolidation'!$B3:$AQ3,'Pre ISIC Consolidation'!$B$26:$AQ$26,FtPICM!B$1)</f>
@@ -4415,7 +4748,7 @@
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4">
         <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$26:$AQ$26,FtPICM!B$1)</f>
@@ -4425,9 +4758,9 @@
         <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$26:$AQ$26,FtPICM!C$1)</f>
         <v>0</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="13">
         <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$26:$AQ$26,FtPICM!D$1)</f>
-        <v>0</v>
+        <v>0.80967342075391113</v>
       </c>
       <c r="E4">
         <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$26:$AQ$26,FtPICM!E$1)</f>
@@ -4517,9 +4850,9 @@
         <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$26:$AQ$26,FtPICM!Z$1)</f>
         <v>0</v>
       </c>
-      <c r="AA4" s="4">
+      <c r="AA4" s="13">
         <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$26:$AQ$26,FtPICM!AA$1)</f>
-        <v>1</v>
+        <v>0.19032657924608889</v>
       </c>
       <c r="AB4">
         <f>SUMIFS('Pre ISIC Consolidation'!$B4:$AQ4,'Pre ISIC Consolidation'!$B$26:$AQ$26,FtPICM!AB$1)</f>
@@ -4588,7 +4921,7 @@
     </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5">
         <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$26:$AQ$26,FtPICM!B$1)</f>
@@ -4602,7 +4935,7 @@
         <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$26:$AQ$26,FtPICM!D$1)</f>
         <v>0</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5">
         <f>SUMIFS('Pre ISIC Consolidation'!$B5:$AQ5,'Pre ISIC Consolidation'!$B$26:$AQ$26,FtPICM!E$1)</f>
         <v>1</v>
       </c>
@@ -4761,7 +5094,7 @@
     </row>
     <row r="6" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6">
         <f>SUMIFS('Pre ISIC Consolidation'!$B6:$AQ6,'Pre ISIC Consolidation'!$B$26:$AQ$26,FtPICM!B$1)</f>
@@ -4934,7 +5267,7 @@
     </row>
     <row r="7" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7">
         <f>SUMIFS('Pre ISIC Consolidation'!$B7:$AQ7,'Pre ISIC Consolidation'!$B$26:$AQ$26,FtPICM!B$1)</f>
@@ -5107,7 +5440,7 @@
     </row>
     <row r="8" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8">
         <f>SUMIFS('Pre ISIC Consolidation'!$B8:$AQ8,'Pre ISIC Consolidation'!$B$26:$AQ$26,FtPICM!B$1)</f>
@@ -5280,7 +5613,7 @@
     </row>
     <row r="9" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9" s="4">
         <f>SUMIFS('Pre ISIC Consolidation'!$B9:$AQ9,'Pre ISIC Consolidation'!$B$26:$AQ$26,FtPICM!B$1)</f>
@@ -5453,7 +5786,7 @@
     </row>
     <row r="10" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10">
         <f>SUMIFS('Pre ISIC Consolidation'!$B10:$AQ10,'Pre ISIC Consolidation'!$B$26:$AQ$26,FtPICM!B$1)</f>
@@ -5626,7 +5959,7 @@
     </row>
     <row r="11" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11">
         <f>SUMIFS('Pre ISIC Consolidation'!$B11:$AQ11,'Pre ISIC Consolidation'!$B$26:$AQ$26,FtPICM!B$1)</f>
@@ -5799,7 +6132,7 @@
     </row>
     <row r="12" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B12">
         <f>SUMIFS('Pre ISIC Consolidation'!$B12:$AQ12,'Pre ISIC Consolidation'!$B$26:$AQ$26,FtPICM!B$1)</f>
@@ -5972,7 +6305,7 @@
     </row>
     <row r="13" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B13">
         <f>SUMIFS('Pre ISIC Consolidation'!$B13:$AQ13,'Pre ISIC Consolidation'!$B$26:$AQ$26,FtPICM!B$1)</f>
@@ -6145,7 +6478,7 @@
     </row>
     <row r="14" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B14">
         <f>SUMIFS('Pre ISIC Consolidation'!$B14:$AQ14,'Pre ISIC Consolidation'!$B$26:$AQ$26,FtPICM!B$1)</f>
@@ -6318,7 +6651,7 @@
     </row>
     <row r="15" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B15">
         <f>SUMIFS('Pre ISIC Consolidation'!$B15:$AQ15,'Pre ISIC Consolidation'!$B$26:$AQ$26,FtPICM!B$1)</f>
@@ -6491,7 +6824,7 @@
     </row>
     <row r="16" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B16">
         <f>SUMIFS('Pre ISIC Consolidation'!$B16:$AQ16,'Pre ISIC Consolidation'!$B$26:$AQ$26,FtPICM!B$1)</f>
@@ -6664,7 +6997,7 @@
     </row>
     <row r="17" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B17">
         <f>SUMIFS('Pre ISIC Consolidation'!$B17:$AQ17,'Pre ISIC Consolidation'!$B$26:$AQ$26,FtPICM!B$1)</f>
@@ -6837,7 +7170,7 @@
     </row>
     <row r="18" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B18">
         <f>SUMIFS('Pre ISIC Consolidation'!$B18:$AQ18,'Pre ISIC Consolidation'!$B$26:$AQ$26,FtPICM!B$1)</f>
@@ -7010,7 +7343,7 @@
     </row>
     <row r="19" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B19">
         <f>SUMIFS('Pre ISIC Consolidation'!$B19:$AQ19,'Pre ISIC Consolidation'!$B$26:$AQ$26,FtPICM!B$1)</f>
@@ -7183,7 +7516,7 @@
     </row>
     <row r="20" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B20">
         <f>SUMIFS('Pre ISIC Consolidation'!$B20:$AQ20,'Pre ISIC Consolidation'!$B$26:$AQ$26,FtPICM!B$1)</f>
@@ -7356,7 +7689,7 @@
     </row>
     <row r="21" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B21">
         <f>SUMIFS('Pre ISIC Consolidation'!$B21:$AQ21,'Pre ISIC Consolidation'!$B$26:$AQ$26,FtPICM!B$1)</f>
@@ -7529,7 +7862,7 @@
     </row>
     <row r="22" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B22">
         <f>SUMIFS('Pre ISIC Consolidation'!$B22:$AQ22,'Pre ISIC Consolidation'!$B$26:$AQ$26,FtPICM!B$1)</f>

</xml_diff>